<commit_message>
added new comp design
comp design for marco's approval/change.
</commit_message>
<xml_diff>
--- a/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
+++ b/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\01_DesignStudio3\00_Project\DS3-WorkInProgress\Docs\00_SCRUM_Files\01_Milestone1\WorkInProgress_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zara Tooth\Desktop\Carleton\Third Year\Semester 2\Design Studio 3\DS3-WorkInProgress\Docs\00_SCRUM_Files\01_Milestone1\WorkInProgress_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -491,13 +491,13 @@
     <t>take initial mockup and finalize it for implementation</t>
   </si>
   <si>
-    <t>Designer approval of final scnene designs</t>
-  </si>
-  <si>
     <t>3 -&gt; 6</t>
   </si>
   <si>
     <t>ensure final scene design fir with project and are at an acceptable level of goodness</t>
+  </si>
+  <si>
+    <t>Designer approval of final scene designs</t>
   </si>
 </sst>
 </file>
@@ -1224,11 +1224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="181514448"/>
-        <c:axId val="349483424"/>
+        <c:axId val="344338040"/>
+        <c:axId val="344338432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="181514448"/>
+        <c:axId val="344338040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1302,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="349483424"/>
+        <c:crossAx val="344338432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1312,7 +1312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="349483424"/>
+        <c:axId val="344338432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1398,7 +1398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181514448"/>
+        <c:crossAx val="344338040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1884,8 +1884,8 @@
   <dimension ref="A1:AT183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15:D16"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2767,22 +2767,25 @@
         <v>36</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
-      <c r="I23" s="6" t="str">
+      <c r="H23" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="I23" s="6">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="J23" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
@@ -2799,33 +2802,36 @@
         <v>36</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
-      <c r="I24" s="6" t="str">
+      <c r="H24" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="6">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-0.5</v>
       </c>
       <c r="J24" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K24" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="47" t="s">
+      <c r="C25" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Updated sprint log and added doc on SDE, Kin & CV
</commit_message>
<xml_diff>
--- a/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
+++ b/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
@@ -1189,25 +1189,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0196078431372548</c:v>
+                  <c:v>0.98235294117647065</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0196078431372548</c:v>
+                  <c:v>0.98235294117647065</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0196078431372548</c:v>
+                  <c:v>0.98235294117647065</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0196078431372548</c:v>
+                  <c:v>0.98235294117647065</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0196078431372548</c:v>
+                  <c:v>0.98235294117647065</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0196078431372548</c:v>
+                  <c:v>0.98235294117647065</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0196078431372548</c:v>
+                  <c:v>0.98235294117647065</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1224,11 +1224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="344338040"/>
-        <c:axId val="344338432"/>
+        <c:axId val="293076832"/>
+        <c:axId val="293072912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="344338040"/>
+        <c:axId val="293076832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1302,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344338432"/>
+        <c:crossAx val="293072912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1312,7 +1312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="344338432"/>
+        <c:axId val="293072912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1398,7 +1398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="344338040"/>
+        <c:crossAx val="293076832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1883,9 +1883,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2008,25 +2008,28 @@
         <v>46</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G2">
         <v>0.5</v>
       </c>
-      <c r="I2" s="6" t="str">
+      <c r="H2" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="6">
         <f t="shared" ref="I2:I44" si="0">IF(H2&lt;&gt;"",H2-G2,"")</f>
-        <v/>
+        <v>-0.4</v>
       </c>
       <c r="J2" s="6">
         <f t="shared" ref="J2:J44" si="1">IF(H2="",G2,H2)</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="K2" s="7">
         <f t="shared" ref="K2:K44" si="2">J2-SUM(M2:AB2)</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
@@ -2040,25 +2043,28 @@
         <v>47</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>0.5</v>
       </c>
-      <c r="I3" s="6" t="str">
+      <c r="H3" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="I3" s="6">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-0.35</v>
       </c>
       <c r="J3" s="6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="4" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
@@ -2072,25 +2078,28 @@
         <v>48</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G4">
         <v>0.5</v>
       </c>
-      <c r="I4" s="6" t="str">
+      <c r="H4" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="I4" s="6">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-0.2</v>
       </c>
       <c r="J4" s="6">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:46" ht="38.25" x14ac:dyDescent="0.2">
@@ -2107,7 +2116,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -2139,7 +2148,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -2475,7 +2484,7 @@
         <v>35</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -2507,7 +2516,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3209,15 +3218,15 @@
       <c r="H46" s="23"/>
       <c r="I46" s="6">
         <f>SUM(I2:I45)</f>
-        <v>0.5</v>
+        <v>-0.44999999999999996</v>
       </c>
       <c r="J46" s="6">
         <f>SUM(J2:J45)</f>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="K46" s="7">
         <f>SUM(K2:K45)</f>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="L46" s="5"/>
       <c r="N46"/>
@@ -3261,7 +3270,7 @@
       </c>
       <c r="G47" s="25">
         <f>J46</f>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="K47" s="26" t="s">
         <v>23</v>
@@ -3303,7 +3312,7 @@
       </c>
       <c r="G48" s="22">
         <f>G47-G46</f>
-        <v>0.5</v>
+        <v>-0.44999999999999929</v>
       </c>
       <c r="K48" s="26" t="s">
         <v>25</v>
@@ -3345,7 +3354,7 @@
       </c>
       <c r="G49" s="28">
         <f>G47/G46-1</f>
-        <v>1.9607843137254832E-2</v>
+        <v>-1.7647058823529349E-2</v>
       </c>
       <c r="K49" s="26" t="s">
         <v>27</v>
@@ -3353,31 +3362,31 @@
       <c r="L49" s="27"/>
       <c r="M49" s="22">
         <f t="shared" ref="M49:S49" si="5">$G47-M48</f>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="N49" s="22">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="O49" s="22">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="P49" s="22">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="Q49" s="22">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="R49" s="22">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="S49" s="22">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>25.05</v>
       </c>
     </row>
     <row r="50" spans="2:35" x14ac:dyDescent="0.2">
@@ -3392,31 +3401,31 @@
       </c>
       <c r="M50" s="30">
         <f t="shared" ref="M50:S50" si="6">M49/$G$46</f>
-        <v>1.0196078431372548</v>
+        <v>0.98235294117647065</v>
       </c>
       <c r="N50" s="30">
         <f t="shared" si="6"/>
-        <v>1.0196078431372548</v>
+        <v>0.98235294117647065</v>
       </c>
       <c r="O50" s="30">
         <f t="shared" si="6"/>
-        <v>1.0196078431372548</v>
+        <v>0.98235294117647065</v>
       </c>
       <c r="P50" s="30">
         <f t="shared" si="6"/>
-        <v>1.0196078431372548</v>
+        <v>0.98235294117647065</v>
       </c>
       <c r="Q50" s="30">
         <f t="shared" si="6"/>
-        <v>1.0196078431372548</v>
+        <v>0.98235294117647065</v>
       </c>
       <c r="R50" s="30">
         <f t="shared" si="6"/>
-        <v>1.0196078431372548</v>
+        <v>0.98235294117647065</v>
       </c>
       <c r="S50" s="30">
         <f t="shared" si="6"/>
-        <v>1.0196078431372548</v>
+        <v>0.98235294117647065</v>
       </c>
       <c r="T50" s="30"/>
       <c r="U50" s="30"/>
@@ -3442,7 +3451,7 @@
       </c>
       <c r="G51" s="22">
         <f>K46</f>
-        <v>26</v>
+        <v>25.05</v>
       </c>
       <c r="M51" s="30"/>
       <c r="N51" s="30"/>
@@ -3499,7 +3508,7 @@
       </c>
       <c r="G55" s="32">
         <f>((G51/G54)/8)/0.8</f>
-        <v>1.015625</v>
+        <v>0.978515625</v>
       </c>
       <c r="J55" s="33"/>
     </row>

</xml_diff>

<commit_message>
Added hours per day of week
Added hours per day of week into sprint sheet
</commit_message>
<xml_diff>
--- a/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
+++ b/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zara Tooth\Desktop\Carleton\Third Year\Semester 2\Design Studio 3\DS3-WorkInProgress\Docs\00_SCRUM_Files\01_Milestone1\WorkInProgress_1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="1980" windowHeight="17565"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
     <definedName name="Team">Lookups!$C$2:$C$7</definedName>
     <definedName name="Type">Lookups!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -37,7 +32,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -190,7 +185,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -238,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1044,7 +1039,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1189,25 +1184,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98235294117647065</c:v>
+                  <c:v>0.90392156862745099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98235294117647065</c:v>
+                  <c:v>0.86470588235294121</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98235294117647065</c:v>
+                  <c:v>0.86470588235294121</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98235294117647065</c:v>
+                  <c:v>0.86470588235294121</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.98235294117647065</c:v>
+                  <c:v>0.82549019607843144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.98235294117647065</c:v>
+                  <c:v>0.82549019607843144</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.98235294117647065</c:v>
+                  <c:v>0.82549019607843144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1224,11 +1219,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="293076832"/>
-        <c:axId val="293072912"/>
+        <c:axId val="211151872"/>
+        <c:axId val="211063552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="293076832"/>
+        <c:axId val="211151872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1302,7 +1297,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293072912"/>
+        <c:crossAx val="211063552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1312,7 +1307,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="293072912"/>
+        <c:axId val="211063552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1398,7 +1393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="293076832"/>
+        <c:crossAx val="211151872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1873,7 +1868,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1884,8 +1879,8 @@
   <dimension ref="A1:AT183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2131,6 +2126,9 @@
       </c>
       <c r="K5" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>0.5</v>
       </c>
     </row>
@@ -2163,6 +2161,9 @@
       </c>
       <c r="K6" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>0.5</v>
       </c>
     </row>
@@ -2426,9 +2427,12 @@
       </c>
       <c r="K13" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
         <v>0.5</v>
       </c>
-      <c r="L13" s="5">
+      <c r="N13">
         <v>0.5</v>
       </c>
     </row>
@@ -2464,9 +2468,12 @@
       </c>
       <c r="K14" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
         <v>0.5</v>
       </c>
-      <c r="L14" s="5">
+      <c r="N14">
         <v>0.5</v>
       </c>
     </row>
@@ -2534,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -2572,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -2610,7 +2617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
@@ -2642,13 +2649,16 @@
       </c>
       <c r="K19" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="M19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -2680,13 +2690,16 @@
       </c>
       <c r="K20" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="M20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
@@ -2724,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -2762,7 +2775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -2797,7 +2810,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -2832,7 +2845,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
@@ -2867,7 +2880,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B26" s="49"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
@@ -2884,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B27" s="49"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
@@ -2901,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" s="49"/>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
@@ -2918,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="49"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
@@ -2935,7 +2948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="49"/>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
@@ -2952,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31" s="49"/>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
@@ -2969,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B32" s="49"/>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
@@ -3226,7 +3239,7 @@
       </c>
       <c r="K46" s="7">
         <f>SUM(K2:K45)</f>
-        <v>25.05</v>
+        <v>21.05</v>
       </c>
       <c r="L46" s="5"/>
       <c r="N46"/>
@@ -3278,11 +3291,11 @@
       <c r="L47" s="27"/>
       <c r="M47" s="22">
         <f t="shared" ref="M47:S47" si="3">SUM(M2:M45)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N47" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O47" s="22">
         <f t="shared" si="3"/>
@@ -3294,7 +3307,7 @@
       </c>
       <c r="Q47" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R47" s="22">
         <f t="shared" si="3"/>
@@ -3320,31 +3333,31 @@
       <c r="L48" s="27"/>
       <c r="M48" s="22">
         <f t="shared" ref="M48:S48" si="4">L48+M47</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N48" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O48" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P48" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q48" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R48" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S48" s="22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:35" x14ac:dyDescent="0.2">
@@ -3362,31 +3375,31 @@
       <c r="L49" s="27"/>
       <c r="M49" s="22">
         <f t="shared" ref="M49:S49" si="5">$G47-M48</f>
-        <v>25.05</v>
+        <v>23.05</v>
       </c>
       <c r="N49" s="22">
         <f t="shared" si="5"/>
-        <v>25.05</v>
+        <v>22.05</v>
       </c>
       <c r="O49" s="22">
         <f t="shared" si="5"/>
-        <v>25.05</v>
+        <v>22.05</v>
       </c>
       <c r="P49" s="22">
         <f t="shared" si="5"/>
-        <v>25.05</v>
+        <v>22.05</v>
       </c>
       <c r="Q49" s="22">
         <f t="shared" si="5"/>
-        <v>25.05</v>
+        <v>21.05</v>
       </c>
       <c r="R49" s="22">
         <f t="shared" si="5"/>
-        <v>25.05</v>
+        <v>21.05</v>
       </c>
       <c r="S49" s="22">
         <f t="shared" si="5"/>
-        <v>25.05</v>
+        <v>21.05</v>
       </c>
     </row>
     <row r="50" spans="2:35" x14ac:dyDescent="0.2">
@@ -3401,31 +3414,31 @@
       </c>
       <c r="M50" s="30">
         <f t="shared" ref="M50:S50" si="6">M49/$G$46</f>
-        <v>0.98235294117647065</v>
+        <v>0.90392156862745099</v>
       </c>
       <c r="N50" s="30">
         <f t="shared" si="6"/>
-        <v>0.98235294117647065</v>
+        <v>0.86470588235294121</v>
       </c>
       <c r="O50" s="30">
         <f t="shared" si="6"/>
-        <v>0.98235294117647065</v>
+        <v>0.86470588235294121</v>
       </c>
       <c r="P50" s="30">
         <f t="shared" si="6"/>
-        <v>0.98235294117647065</v>
+        <v>0.86470588235294121</v>
       </c>
       <c r="Q50" s="30">
         <f t="shared" si="6"/>
-        <v>0.98235294117647065</v>
+        <v>0.82549019607843144</v>
       </c>
       <c r="R50" s="30">
         <f t="shared" si="6"/>
-        <v>0.98235294117647065</v>
+        <v>0.82549019607843144</v>
       </c>
       <c r="S50" s="30">
         <f t="shared" si="6"/>
-        <v>0.98235294117647065</v>
+        <v>0.82549019607843144</v>
       </c>
       <c r="T50" s="30"/>
       <c r="U50" s="30"/>
@@ -3451,7 +3464,7 @@
       </c>
       <c r="G51" s="22">
         <f>K46</f>
-        <v>25.05</v>
+        <v>21.05</v>
       </c>
       <c r="M51" s="30"/>
       <c r="N51" s="30"/>
@@ -3483,7 +3496,7 @@
       </c>
       <c r="G52" s="28">
         <f>G51/G47</f>
-        <v>1</v>
+        <v>0.84031936127744511</v>
       </c>
       <c r="K52" s="26"/>
       <c r="L52"/>
@@ -3508,7 +3521,7 @@
       </c>
       <c r="G55" s="32">
         <f>((G51/G54)/8)/0.8</f>
-        <v>0.978515625</v>
+        <v>0.822265625</v>
       </c>
       <c r="J55" s="33"/>
     </row>

</xml_diff>

<commit_message>
added hours per day of week again
</commit_message>
<xml_diff>
--- a/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
+++ b/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zara Tooth\Desktop\Carleton\Third Year\Semester 2\Design Studio 3\DS3-WorkInProgress\Docs\00_SCRUM_Files\01_Milestone1\WorkInProgress_1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="1980" windowHeight="17565"/>
   </bookViews>
@@ -22,7 +27,7 @@
     <definedName name="Team">Lookups!$C$2:$C$7</definedName>
     <definedName name="Type">Lookups!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -32,7 +37,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -45,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +190,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -209,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -233,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1039,7 +1044,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1184,25 +1189,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90392156862745099</c:v>
+                  <c:v>0.78627450980392155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.86470588235294121</c:v>
+                  <c:v>0.66862745098039222</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86470588235294121</c:v>
+                  <c:v>0.66862745098039222</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86470588235294121</c:v>
+                  <c:v>0.66862745098039222</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82549019607843144</c:v>
+                  <c:v>0.62941176470588234</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.82549019607843144</c:v>
+                  <c:v>0.60784313725490191</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.82549019607843144</c:v>
+                  <c:v>0.60784313725490191</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1219,11 +1224,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="211151872"/>
-        <c:axId val="211063552"/>
+        <c:axId val="228835160"/>
+        <c:axId val="228835552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="211151872"/>
+        <c:axId val="228835160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1297,7 +1302,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211063552"/>
+        <c:crossAx val="228835552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1307,7 +1312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="211063552"/>
+        <c:axId val="228835552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -1393,7 +1398,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211151872"/>
+        <c:crossAx val="228835160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1868,7 +1873,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1879,8 +1884,8 @@
   <dimension ref="A1:AT183"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2024,6 +2029,9 @@
       </c>
       <c r="K2" s="7">
         <f t="shared" ref="K2:K44" si="2">J2-SUM(M2:AB2)</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="5">
         <v>0.1</v>
       </c>
     </row>
@@ -2059,6 +2067,9 @@
       </c>
       <c r="K3" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
         <v>0.15</v>
       </c>
     </row>
@@ -2094,6 +2105,9 @@
       </c>
       <c r="K4" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
         <v>0.3</v>
       </c>
     </row>
@@ -2275,9 +2289,12 @@
       </c>
       <c r="K9" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="5">
         <v>2</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M9" s="3">
         <v>2</v>
       </c>
     </row>
@@ -2313,9 +2330,12 @@
       </c>
       <c r="K10" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="5">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2541,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -2579,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -2617,7 +2637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>64</v>
       </c>
@@ -2658,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
@@ -2699,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
@@ -2737,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -2775,7 +2795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -2807,10 +2827,13 @@
       </c>
       <c r="K23" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N23">
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -2842,10 +2865,13 @@
       </c>
       <c r="K24" s="7">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>74</v>
       </c>
@@ -2880,7 +2906,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B26" s="49"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
@@ -2897,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B27" s="49"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
@@ -2914,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B28" s="49"/>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
@@ -2931,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B29" s="49"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
@@ -2948,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B30" s="49"/>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
@@ -2965,7 +2991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B31" s="49"/>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
@@ -2982,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B32" s="49"/>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
@@ -3239,7 +3265,7 @@
       </c>
       <c r="K46" s="7">
         <f>SUM(K2:K45)</f>
-        <v>21.05</v>
+        <v>15.5</v>
       </c>
       <c r="L46" s="5"/>
       <c r="N46"/>
@@ -3291,11 +3317,11 @@
       <c r="L47" s="27"/>
       <c r="M47" s="22">
         <f t="shared" ref="M47:S47" si="3">SUM(M2:M45)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N47" s="22">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O47" s="22">
         <f t="shared" si="3"/>
@@ -3311,7 +3337,7 @@
       </c>
       <c r="R47" s="22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S47" s="22">
         <f t="shared" si="3"/>
@@ -3333,31 +3359,31 @@
       <c r="L48" s="27"/>
       <c r="M48" s="22">
         <f t="shared" ref="M48:S48" si="4">L48+M47</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N48" s="22">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O48" s="22">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="P48" s="22">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="Q48" s="22">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="R48" s="22">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="S48" s="22">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="49" spans="2:35" x14ac:dyDescent="0.2">
@@ -3375,31 +3401,31 @@
       <c r="L49" s="27"/>
       <c r="M49" s="22">
         <f t="shared" ref="M49:S49" si="5">$G47-M48</f>
-        <v>23.05</v>
+        <v>20.05</v>
       </c>
       <c r="N49" s="22">
         <f t="shared" si="5"/>
-        <v>22.05</v>
+        <v>17.05</v>
       </c>
       <c r="O49" s="22">
         <f t="shared" si="5"/>
-        <v>22.05</v>
+        <v>17.05</v>
       </c>
       <c r="P49" s="22">
         <f t="shared" si="5"/>
-        <v>22.05</v>
+        <v>17.05</v>
       </c>
       <c r="Q49" s="22">
         <f t="shared" si="5"/>
-        <v>21.05</v>
+        <v>16.05</v>
       </c>
       <c r="R49" s="22">
         <f t="shared" si="5"/>
-        <v>21.05</v>
+        <v>15.5</v>
       </c>
       <c r="S49" s="22">
         <f t="shared" si="5"/>
-        <v>21.05</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="50" spans="2:35" x14ac:dyDescent="0.2">
@@ -3414,31 +3440,31 @@
       </c>
       <c r="M50" s="30">
         <f t="shared" ref="M50:S50" si="6">M49/$G$46</f>
-        <v>0.90392156862745099</v>
+        <v>0.78627450980392155</v>
       </c>
       <c r="N50" s="30">
         <f t="shared" si="6"/>
-        <v>0.86470588235294121</v>
+        <v>0.66862745098039222</v>
       </c>
       <c r="O50" s="30">
         <f t="shared" si="6"/>
-        <v>0.86470588235294121</v>
+        <v>0.66862745098039222</v>
       </c>
       <c r="P50" s="30">
         <f t="shared" si="6"/>
-        <v>0.86470588235294121</v>
+        <v>0.66862745098039222</v>
       </c>
       <c r="Q50" s="30">
         <f t="shared" si="6"/>
-        <v>0.82549019607843144</v>
+        <v>0.62941176470588234</v>
       </c>
       <c r="R50" s="30">
         <f t="shared" si="6"/>
-        <v>0.82549019607843144</v>
+        <v>0.60784313725490191</v>
       </c>
       <c r="S50" s="30">
         <f t="shared" si="6"/>
-        <v>0.82549019607843144</v>
+        <v>0.60784313725490191</v>
       </c>
       <c r="T50" s="30"/>
       <c r="U50" s="30"/>
@@ -3464,7 +3490,7 @@
       </c>
       <c r="G51" s="22">
         <f>K46</f>
-        <v>21.05</v>
+        <v>15.5</v>
       </c>
       <c r="M51" s="30"/>
       <c r="N51" s="30"/>
@@ -3496,7 +3522,7 @@
       </c>
       <c r="G52" s="28">
         <f>G51/G47</f>
-        <v>0.84031936127744511</v>
+        <v>0.61876247504990023</v>
       </c>
       <c r="K52" s="26"/>
       <c r="L52"/>
@@ -3521,7 +3547,7 @@
       </c>
       <c r="G55" s="32">
         <f>((G51/G54)/8)/0.8</f>
-        <v>0.822265625</v>
+        <v>0.60546875</v>
       </c>
       <c r="J55" s="33"/>
     </row>

</xml_diff>

<commit_message>
updated Marco Folder for SCRUM
</commit_message>
<xml_diff>
--- a/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
+++ b/Docs/00_SCRUM_Files/01_Milestone1/WorkInProgress_1/WorkInProgress_1.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zara Tooth\Desktop\Carleton\Third Year\Semester 2\Design Studio 3\DS3-WorkInProgress\Docs\00_SCRUM_Files\01_Milestone1\WorkInProgress_1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="1980" windowHeight="17565"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="15400"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,12 @@
     <definedName name="Team">Lookups!$C$2:$C$7</definedName>
     <definedName name="Type">Lookups!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="130407"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -37,7 +37,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -50,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -128,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -190,7 +190,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -214,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -238,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -270,6 +270,87 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="75">
   <si>
+    <t>based on project needs, decide which computer vision library will work best</t>
+  </si>
+  <si>
+    <t>Decide what kind of computer will be needed to run / render our final design</t>
+  </si>
+  <si>
+    <t>Decide what equipment will be needed to complete the installation (projector, screen etc)</t>
+  </si>
+  <si>
+    <t>Create sketches/preliminary mock-ups for design</t>
+  </si>
+  <si>
+    <t>figure out how user interaction affects the scene</t>
+  </si>
+  <si>
+    <t>Create running OpenFrameworks project</t>
+  </si>
+  <si>
+    <t>create diagrams etc to describe effective code/class layout for project</t>
+  </si>
+  <si>
+    <t>Mockup look for first scene</t>
+  </si>
+  <si>
+    <t>Mockup interaction for first scene</t>
+  </si>
+  <si>
+    <t>Mockup look for second scene</t>
+  </si>
+  <si>
+    <t>Mockup interaction for second scene</t>
+  </si>
+  <si>
+    <t>Mockup look for third scene</t>
+  </si>
+  <si>
+    <t>Mockup interaction for third scene</t>
+  </si>
+  <si>
+    <t>Mockup look for fourth</t>
+  </si>
+  <si>
+    <t>Mockup interaction for fourth scene</t>
+  </si>
+  <si>
+    <t>Final design for first scene</t>
+  </si>
+  <si>
+    <t>Final design for second scene</t>
+  </si>
+  <si>
+    <t>final interaction design for second  scene</t>
+  </si>
+  <si>
+    <t>final interaction design for first scene</t>
+  </si>
+  <si>
+    <t>Final design for third scene</t>
+  </si>
+  <si>
+    <t>final interaction design for third scenen</t>
+  </si>
+  <si>
+    <t>Final design for fourth scene</t>
+  </si>
+  <si>
+    <t>final interaction design for fourth scene</t>
+  </si>
+  <si>
+    <t>take initial mockup and finalize it for implementation</t>
+  </si>
+  <si>
+    <t>3 -&gt; 6</t>
+  </si>
+  <si>
+    <t>ensure final scene design fir with project and are at an acceptable level of goodness</t>
+  </si>
+  <si>
+    <t>Designer approval of final scene designs</t>
+  </si>
+  <si>
     <t>Tasks</t>
   </si>
   <si>
@@ -417,98 +498,17 @@
   </si>
   <si>
     <t>based on project needs, decide which Kinect library will work best</t>
-  </si>
-  <si>
-    <t>based on project needs, decide which computer vision library will work best</t>
-  </si>
-  <si>
-    <t>Decide what kind of computer will be needed to run / render our final design</t>
-  </si>
-  <si>
-    <t>Decide what equipment will be needed to complete the installation (projector, screen etc)</t>
-  </si>
-  <si>
-    <t>Create sketches/preliminary mock-ups for design</t>
-  </si>
-  <si>
-    <t>figure out how user interaction affects the scene</t>
-  </si>
-  <si>
-    <t>Create running OpenFrameworks project</t>
-  </si>
-  <si>
-    <t>create diagrams etc to describe effective code/class layout for project</t>
-  </si>
-  <si>
-    <t>Mockup look for first scene</t>
-  </si>
-  <si>
-    <t>Mockup interaction for first scene</t>
-  </si>
-  <si>
-    <t>Mockup look for second scene</t>
-  </si>
-  <si>
-    <t>Mockup interaction for second scene</t>
-  </si>
-  <si>
-    <t>Mockup look for third scene</t>
-  </si>
-  <si>
-    <t>Mockup interaction for third scene</t>
-  </si>
-  <si>
-    <t>Mockup look for fourth</t>
-  </si>
-  <si>
-    <t>Mockup interaction for fourth scene</t>
-  </si>
-  <si>
-    <t>Final design for first scene</t>
-  </si>
-  <si>
-    <t>Final design for second scene</t>
-  </si>
-  <si>
-    <t>final interaction design for second  scene</t>
-  </si>
-  <si>
-    <t>final interaction design for first scene</t>
-  </si>
-  <si>
-    <t>Final design for third scene</t>
-  </si>
-  <si>
-    <t>final interaction design for third scenen</t>
-  </si>
-  <si>
-    <t>Final design for fourth scene</t>
-  </si>
-  <si>
-    <t>final interaction design for fourth scene</t>
-  </si>
-  <si>
-    <t>take initial mockup and finalize it for implementation</t>
-  </si>
-  <si>
-    <t>3 -&gt; 6</t>
-  </si>
-  <si>
-    <t>ensure final scene design fir with project and are at an acceptable level of goodness</t>
-  </si>
-  <si>
-    <t>Designer approval of final scene designs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -554,9 +554,13 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="0"/>
+      <color indexed="9"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="6">
@@ -961,7 +965,7 @@
       </border>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1043,17 +1047,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1082,11 +1077,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.33459712272808007"/>
-          <c:y val="2.6882567098467532E-2"/>
+          <c:x val="0.33459712272808"/>
+          <c:y val="0.0268825670984675"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -1094,22 +1088,20 @@
         </a:ln>
       </c:spPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1381622881186185"/>
-          <c:y val="0.15457489292864876"/>
-          <c:w val="0.84871119844294207"/>
-          <c:h val="0.69088256491587363"/>
+          <c:x val="0.138162288118618"/>
+          <c:y val="0.154574892928649"/>
+          <c:w val="0.848711198442942"/>
+          <c:h val="0.690882564915874"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1186,53 +1178,42 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78627450980392155</c:v>
+                  <c:v>0.825490196078431</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66862745098039222</c:v>
+                  <c:v>0.550980392156863</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66862745098039222</c:v>
+                  <c:v>0.550980392156863</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66862745098039222</c:v>
+                  <c:v>0.550980392156863</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.62941176470588234</c:v>
+                  <c:v>0.433333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60784313725490191</c:v>
+                  <c:v>0.411764705882353</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.60784313725490191</c:v>
+                  <c:v>0.411764705882353</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="228835160"/>
-        <c:axId val="228835552"/>
+        <c:axId val="431532488"/>
+        <c:axId val="431540344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="228835160"/>
+        <c:axId val="431532488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1261,11 +1242,10 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.51035452805241455"/>
-              <c:y val="0.92207278525668168"/>
+              <c:x val="0.510354528052414"/>
+              <c:y val="0.922072785256682"/>
             </c:manualLayout>
           </c:layout>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1274,8 +1254,6 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:spPr>
           <a:ln w="3175">
@@ -1302,23 +1280,21 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228835552"/>
+        <c:crossAx val="431540344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:tickLblSkip val="2"/>
         <c:tickMarkSkip val="1"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228835552"/>
+        <c:axId val="431540344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
-          <c:min val="0"/>
+          <c:min val="0.0"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1357,11 +1333,10 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.5038087344345115E-2"/>
-              <c:y val="0.34947365450286461"/>
+              <c:x val="0.0150380873443451"/>
+              <c:y val="0.349473654502865"/>
             </c:manualLayout>
           </c:layout>
-          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln w="25400">
@@ -1370,8 +1345,6 @@
           </c:spPr>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:spPr>
           <a:ln w="3175">
@@ -1398,7 +1371,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228835160"/>
+        <c:crossAx val="431532488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1420,13 +1393,12 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.76224231839441126"/>
-          <c:y val="4.9732735021025598E-2"/>
-          <c:w val="0.18797594379649907"/>
-          <c:h val="4.7044562978014848E-2"/>
+          <c:x val="0.762242318394411"/>
+          <c:y val="0.0497327350210256"/>
+          <c:w val="0.187975943796499"/>
+          <c:h val="0.0470445629780148"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
@@ -1456,9 +1428,7 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="0"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1490,7 +1460,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.51180555555555551" footer="0.51180555555555551"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.511805555555556" footer="0.511805555555556"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1576,7 +1546,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1611,7 +1581,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1800,11 +1770,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1814,7 +1784,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1842,11 +1812,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1856,7 +1826,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1873,101 +1843,101 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AT183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="52" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="6"/>
+    <col min="1" max="1" width="23.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="52" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="6"/>
     <col min="10" max="10" width="11" style="6" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="7" customWidth="1"/>
     <col min="12" max="12" width="9" style="5" customWidth="1"/>
     <col min="13" max="13" width="9" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
-    <col min="15" max="16" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="15" max="16" width="10.1640625" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" customWidth="1"/>
     <col min="19" max="19" width="12" customWidth="1"/>
-    <col min="20" max="35" width="10.140625" customWidth="1"/>
+    <col min="20" max="35" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="39" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" s="39" customFormat="1" ht="40.5" customHeight="1">
       <c r="A1" s="42" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F1" s="43" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="K1" s="46" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="L1" s="44" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="M1" s="44" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="N1" s="44" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="O1" s="44" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="P1" s="44" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="44" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="R1" s="44" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="S1" s="44" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="T1" s="41"/>
       <c r="U1" s="41"/>
@@ -1997,21 +1967,21 @@
       <c r="AS1" s="40"/>
       <c r="AT1" s="40"/>
     </row>
-    <row r="2" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" ht="24">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="B2" s="49">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>19</v>
       </c>
       <c r="G2">
         <v>0.5</v>
@@ -2035,21 +2005,21 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:46" ht="24">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="B3" s="49">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G3">
         <v>0.5</v>
@@ -2073,21 +2043,21 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:46" ht="24">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B4" s="49">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G4">
         <v>0.5</v>
@@ -2111,21 +2081,21 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" ht="36">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B5" s="49">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -2146,21 +2116,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:46" ht="41.25" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B6" s="49">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -2181,21 +2151,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:46" ht="24">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="B7" s="49">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -2219,21 +2189,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:46" ht="24">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="B8" s="49">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G8">
         <v>0.5</v>
@@ -2257,21 +2227,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:46" ht="24">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B9" s="49">
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -2298,21 +2268,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:46" ht="24">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="B10" s="49">
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G10">
         <v>0.5</v>
@@ -2339,21 +2309,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:46" ht="24">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B11" s="49">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -2371,27 +2341,30 @@
       </c>
       <c r="K11" s="7">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" ht="24">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="B12" s="49">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G12">
         <v>0.5</v>
@@ -2409,27 +2382,30 @@
       </c>
       <c r="K12" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:46" ht="24">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B13" s="49">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -2456,21 +2432,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:46" ht="24">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="B14" s="49">
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G14">
         <v>0.5</v>
@@ -2497,21 +2473,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:46" ht="24">
       <c r="A15" s="1" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="B15" s="49">
         <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -2529,21 +2505,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:46" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:46" ht="24">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="B16" s="49">
         <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -2561,21 +2537,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" ht="24">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="B17" s="49">
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -2599,21 +2575,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="24">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B18" s="49">
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2637,21 +2613,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="24">
       <c r="A19" s="1" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="B19" s="49">
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -2678,21 +2654,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="24">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B20" s="49">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -2719,21 +2695,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="24">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="B21" s="49">
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -2751,27 +2727,30 @@
       </c>
       <c r="K21" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="24">
       <c r="A22" s="1" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="B22" s="49">
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2789,27 +2768,30 @@
       </c>
       <c r="K22" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L22" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="N22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="24">
       <c r="A23" s="1" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="B23" s="49">
         <v>6</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2833,21 +2815,21 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="24">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="B24" s="49">
         <v>6</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -2871,42 +2853,48 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="24">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="B25" s="47" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>20</v>
+        <v>64</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="I25" s="6" t="str">
+      <c r="H25" s="5">
+        <v>2</v>
+      </c>
+      <c r="I25" s="6">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J25" s="6">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" s="7">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="B26" s="49"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
@@ -2923,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17">
       <c r="B27" s="49"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
@@ -2940,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17">
       <c r="B28" s="49"/>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
@@ -2957,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17">
       <c r="B29" s="49"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
@@ -2974,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17">
       <c r="B30" s="49"/>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
@@ -2991,7 +2979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17">
       <c r="B31" s="49"/>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
@@ -3008,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17">
       <c r="B32" s="49"/>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
@@ -3025,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:46">
       <c r="B33" s="49"/>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
@@ -3042,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:46">
       <c r="B34" s="49"/>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
@@ -3059,7 +3047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:46">
       <c r="B35" s="49"/>
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
@@ -3076,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:46">
       <c r="B36" s="49"/>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
@@ -3093,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:46">
       <c r="B37" s="49"/>
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
@@ -3110,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:46">
       <c r="B38" s="49"/>
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
@@ -3127,7 +3115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:46">
       <c r="B39" s="49"/>
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
@@ -3144,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:46">
       <c r="B40" s="49"/>
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
@@ -3161,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:46">
       <c r="B41" s="49"/>
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
@@ -3178,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:46">
       <c r="B42" s="49"/>
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
@@ -3195,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:46">
       <c r="B43" s="49"/>
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
@@ -3212,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:46">
       <c r="B44" s="49"/>
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
@@ -3229,7 +3217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:46" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:46" s="12" customFormat="1">
       <c r="A45" s="10"/>
       <c r="B45" s="50"/>
       <c r="C45" s="10"/>
@@ -3241,14 +3229,14 @@
       <c r="K45" s="17"/>
       <c r="L45" s="14"/>
     </row>
-    <row r="46" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:46" s="3" customFormat="1">
       <c r="A46" s="18"/>
       <c r="B46" s="51"/>
       <c r="C46" s="18"/>
       <c r="D46" s="19"/>
       <c r="E46" s="20"/>
       <c r="F46" s="21" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="G46" s="22">
         <f>SUM(G2:G45)</f>
@@ -3257,15 +3245,15 @@
       <c r="H46" s="23"/>
       <c r="I46" s="6">
         <f>SUM(I2:I45)</f>
-        <v>-0.44999999999999996</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J46" s="6">
         <f>SUM(J2:J45)</f>
-        <v>25.05</v>
+        <v>26.05</v>
       </c>
       <c r="K46" s="7">
         <f>SUM(K2:K45)</f>
-        <v>15.5</v>
+        <v>10.5</v>
       </c>
       <c r="L46" s="5"/>
       <c r="N46"/>
@@ -3302,17 +3290,17 @@
       <c r="AS46"/>
       <c r="AT46"/>
     </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:46">
       <c r="B47" s="49"/>
       <c r="F47" s="24" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="G47" s="25">
         <f>J46</f>
-        <v>25.05</v>
+        <v>26.05</v>
       </c>
       <c r="K47" s="26" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="L47" s="27"/>
       <c r="M47" s="22">
@@ -3321,7 +3309,7 @@
       </c>
       <c r="N47" s="22">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O47" s="22">
         <f t="shared" si="3"/>
@@ -3333,7 +3321,7 @@
       </c>
       <c r="Q47" s="22">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R47" s="22">
         <f t="shared" si="3"/>
@@ -3344,17 +3332,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:46">
       <c r="B48" s="49"/>
       <c r="F48" s="4" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="G48" s="22">
         <f>G47-G46</f>
-        <v>-0.44999999999999929</v>
+        <v>0.55000000000000071</v>
       </c>
       <c r="K48" s="26" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="L48" s="27"/>
       <c r="M48" s="22">
@@ -3363,108 +3351,108 @@
       </c>
       <c r="N48" s="22">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O48" s="22">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="P48" s="22">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Q48" s="22">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="R48" s="22">
         <f t="shared" si="4"/>
-        <v>9.5500000000000007</v>
+        <v>15.55</v>
       </c>
       <c r="S48" s="22">
         <f t="shared" si="4"/>
-        <v>9.5500000000000007</v>
-      </c>
-    </row>
-    <row r="49" spans="2:35" x14ac:dyDescent="0.2">
+        <v>15.55</v>
+      </c>
+    </row>
+    <row r="49" spans="2:35">
       <c r="B49" s="49"/>
       <c r="F49" s="24" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="G49" s="28">
         <f>G47/G46-1</f>
-        <v>-1.7647058823529349E-2</v>
+        <v>2.1568627450980316E-2</v>
       </c>
       <c r="K49" s="26" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="L49" s="27"/>
       <c r="M49" s="22">
         <f t="shared" ref="M49:S49" si="5">$G47-M48</f>
-        <v>20.05</v>
+        <v>21.05</v>
       </c>
       <c r="N49" s="22">
         <f t="shared" si="5"/>
-        <v>17.05</v>
+        <v>14.05</v>
       </c>
       <c r="O49" s="22">
         <f t="shared" si="5"/>
-        <v>17.05</v>
+        <v>14.05</v>
       </c>
       <c r="P49" s="22">
         <f t="shared" si="5"/>
-        <v>17.05</v>
+        <v>14.05</v>
       </c>
       <c r="Q49" s="22">
         <f t="shared" si="5"/>
-        <v>16.05</v>
+        <v>11.05</v>
       </c>
       <c r="R49" s="22">
         <f t="shared" si="5"/>
-        <v>15.5</v>
+        <v>10.5</v>
       </c>
       <c r="S49" s="22">
         <f t="shared" si="5"/>
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="50" spans="2:35" x14ac:dyDescent="0.2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:35">
       <c r="B50" s="49"/>
       <c r="F50" s="24"/>
       <c r="G50" s="25"/>
       <c r="K50" s="26" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="L50" s="29">
         <v>1</v>
       </c>
       <c r="M50" s="30">
         <f t="shared" ref="M50:S50" si="6">M49/$G$46</f>
-        <v>0.78627450980392155</v>
+        <v>0.82549019607843144</v>
       </c>
       <c r="N50" s="30">
         <f t="shared" si="6"/>
-        <v>0.66862745098039222</v>
+        <v>0.55098039215686279</v>
       </c>
       <c r="O50" s="30">
         <f t="shared" si="6"/>
-        <v>0.66862745098039222</v>
+        <v>0.55098039215686279</v>
       </c>
       <c r="P50" s="30">
         <f t="shared" si="6"/>
-        <v>0.66862745098039222</v>
+        <v>0.55098039215686279</v>
       </c>
       <c r="Q50" s="30">
         <f t="shared" si="6"/>
-        <v>0.62941176470588234</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="R50" s="30">
         <f t="shared" si="6"/>
-        <v>0.60784313725490191</v>
+        <v>0.41176470588235292</v>
       </c>
       <c r="S50" s="30">
         <f t="shared" si="6"/>
-        <v>0.60784313725490191</v>
+        <v>0.41176470588235292</v>
       </c>
       <c r="T50" s="30"/>
       <c r="U50" s="30"/>
@@ -3483,14 +3471,14 @@
       <c r="AH50" s="30"/>
       <c r="AI50" s="30"/>
     </row>
-    <row r="51" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:35">
       <c r="B51" s="49"/>
       <c r="F51" s="4" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="G51" s="22">
         <f>K46</f>
-        <v>15.5</v>
+        <v>10.5</v>
       </c>
       <c r="M51" s="30"/>
       <c r="N51" s="30"/>
@@ -3516,465 +3504,466 @@
       <c r="AH51" s="30"/>
       <c r="AI51" s="30"/>
     </row>
-    <row r="52" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:35">
       <c r="F52" s="24" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G52" s="28">
         <f>G51/G47</f>
-        <v>0.61876247504990023</v>
+        <v>0.40307101727447214</v>
       </c>
       <c r="K52" s="26"/>
       <c r="L52"/>
       <c r="M52"/>
     </row>
-    <row r="53" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:35">
       <c r="F53" s="24"/>
       <c r="G53" s="25"/>
     </row>
-    <row r="54" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:35">
       <c r="F54" s="4" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="G54">
         <v>4</v>
       </c>
       <c r="M54" s="31"/>
     </row>
-    <row r="55" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:35">
       <c r="F55" s="24" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="G55" s="32">
         <f>((G51/G54)/8)/0.8</f>
-        <v>0.60546875</v>
+        <v>0.41015625</v>
       </c>
       <c r="J55" s="33"/>
     </row>
-    <row r="56" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:35">
       <c r="J56" s="33"/>
       <c r="K56" s="34"/>
       <c r="L56" s="35"/>
     </row>
-    <row r="58" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:35">
       <c r="K58" s="34"/>
       <c r="L58" s="35"/>
       <c r="O58" s="30"/>
     </row>
-    <row r="68" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="11:12">
       <c r="K68" s="26"/>
       <c r="L68" s="27"/>
     </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:5">
       <c r="D82" s="8"/>
       <c r="E82" s="9"/>
     </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:5">
       <c r="D83" s="8"/>
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:5">
       <c r="D84" s="8"/>
       <c r="E84" s="9"/>
     </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:5">
       <c r="D85" s="8"/>
       <c r="E85" s="9"/>
     </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:5">
       <c r="D86" s="8"/>
       <c r="E86" s="9"/>
     </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:5">
       <c r="D87" s="8"/>
       <c r="E87" s="9"/>
     </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:5">
       <c r="D88" s="8"/>
       <c r="E88" s="9"/>
     </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:5">
       <c r="D89" s="8"/>
       <c r="E89" s="9"/>
     </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:5">
       <c r="D90" s="8"/>
       <c r="E90" s="9"/>
     </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:5">
       <c r="D91" s="8"/>
       <c r="E91" s="9"/>
     </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:5">
       <c r="D92" s="8"/>
       <c r="E92" s="9"/>
     </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:5">
       <c r="D93" s="8"/>
       <c r="E93" s="9"/>
     </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:5">
       <c r="D94" s="8"/>
       <c r="E94" s="9"/>
     </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:5">
       <c r="D95" s="8"/>
       <c r="E95" s="9"/>
     </row>
-    <row r="96" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:5">
       <c r="D96" s="8"/>
       <c r="E96" s="9"/>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:5">
       <c r="D97" s="8"/>
       <c r="E97" s="9"/>
     </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:5">
       <c r="D98" s="8"/>
       <c r="E98" s="9"/>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="4:5">
       <c r="D99" s="8"/>
       <c r="E99" s="9"/>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:5">
       <c r="D100" s="8"/>
       <c r="E100" s="9"/>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:5">
       <c r="D101" s="8"/>
       <c r="E101" s="9"/>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:5">
       <c r="D102" s="8"/>
       <c r="E102" s="9"/>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:5">
       <c r="D103" s="8"/>
       <c r="E103" s="9"/>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:5">
       <c r="D104" s="8"/>
       <c r="E104" s="9"/>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:5">
       <c r="D105" s="8"/>
       <c r="E105" s="9"/>
     </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:5">
       <c r="D106" s="8"/>
       <c r="E106" s="9"/>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:5">
       <c r="D107" s="8"/>
       <c r="E107" s="9"/>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:5">
       <c r="D108" s="8"/>
       <c r="E108" s="9"/>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:5">
       <c r="D109" s="8"/>
       <c r="E109" s="9"/>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:5">
       <c r="D110" s="8"/>
       <c r="E110" s="9"/>
     </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:5">
       <c r="D111" s="8"/>
       <c r="E111" s="9"/>
     </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:5">
       <c r="D112" s="8"/>
       <c r="E112" s="9"/>
     </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:5">
       <c r="D113" s="8"/>
       <c r="E113" s="9"/>
     </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:5">
       <c r="D114" s="8"/>
       <c r="E114" s="9"/>
     </row>
-    <row r="115" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:5">
       <c r="D115" s="8"/>
       <c r="E115" s="9"/>
     </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:5">
       <c r="D116" s="8"/>
       <c r="E116" s="9"/>
     </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:5">
       <c r="D117" s="8"/>
       <c r="E117" s="9"/>
     </row>
-    <row r="118" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:5">
       <c r="D118" s="8"/>
       <c r="E118" s="9"/>
     </row>
-    <row r="119" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="4:5">
       <c r="D119" s="8"/>
       <c r="E119" s="9"/>
     </row>
-    <row r="120" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="4:5">
       <c r="D120" s="8"/>
       <c r="E120" s="9"/>
     </row>
-    <row r="121" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="4:5">
       <c r="D121" s="8"/>
       <c r="E121" s="9"/>
     </row>
-    <row r="122" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="4:5">
       <c r="D122" s="8"/>
       <c r="E122" s="9"/>
     </row>
-    <row r="123" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="4:5">
       <c r="D123" s="8"/>
       <c r="E123" s="9"/>
     </row>
-    <row r="124" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="4:5">
       <c r="D124" s="8"/>
       <c r="E124" s="9"/>
     </row>
-    <row r="125" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="4:5">
       <c r="D125" s="8"/>
       <c r="E125" s="9"/>
     </row>
-    <row r="126" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="4:5">
       <c r="D126" s="8"/>
       <c r="E126" s="9"/>
     </row>
-    <row r="127" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="4:5">
       <c r="D127" s="8"/>
       <c r="E127" s="9"/>
     </row>
-    <row r="128" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="4:5">
       <c r="D128" s="8"/>
       <c r="E128" s="9"/>
     </row>
-    <row r="129" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:5">
       <c r="D129" s="8"/>
       <c r="E129" s="9"/>
     </row>
-    <row r="130" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="4:5">
       <c r="D130" s="8"/>
       <c r="E130" s="9"/>
     </row>
-    <row r="131" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="4:5">
       <c r="D131" s="8"/>
       <c r="E131" s="9"/>
     </row>
-    <row r="132" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="4:5">
       <c r="D132" s="8"/>
       <c r="E132" s="9"/>
     </row>
-    <row r="133" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="4:5">
       <c r="D133" s="8"/>
       <c r="E133" s="9"/>
     </row>
-    <row r="134" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="4:5">
       <c r="D134" s="8"/>
       <c r="E134" s="9"/>
     </row>
-    <row r="135" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="4:5">
       <c r="D135" s="8"/>
       <c r="E135" s="9"/>
     </row>
-    <row r="136" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="4:5">
       <c r="D136" s="8"/>
       <c r="E136" s="9"/>
     </row>
-    <row r="137" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="4:5">
       <c r="D137" s="8"/>
       <c r="E137" s="9"/>
     </row>
-    <row r="138" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="4:5">
       <c r="D138" s="8"/>
       <c r="E138" s="9"/>
     </row>
-    <row r="139" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="4:5">
       <c r="D139" s="8"/>
       <c r="E139" s="9"/>
     </row>
-    <row r="140" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="4:5">
       <c r="D140" s="8"/>
       <c r="E140" s="9"/>
     </row>
-    <row r="141" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="4:5">
       <c r="D141" s="8"/>
       <c r="E141" s="9"/>
     </row>
-    <row r="142" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="4:5">
       <c r="D142" s="8"/>
       <c r="E142" s="9"/>
     </row>
-    <row r="143" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="4:5">
       <c r="D143" s="8"/>
       <c r="E143" s="9"/>
     </row>
-    <row r="144" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="4:5">
       <c r="D144" s="8"/>
       <c r="E144" s="9"/>
     </row>
-    <row r="145" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="4:5">
       <c r="D145" s="8"/>
       <c r="E145" s="9"/>
     </row>
-    <row r="146" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="4:5">
       <c r="D146" s="8"/>
       <c r="E146" s="9"/>
     </row>
-    <row r="147" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="4:5">
       <c r="D147" s="8"/>
       <c r="E147" s="9"/>
     </row>
-    <row r="148" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="4:5">
       <c r="D148" s="8"/>
       <c r="E148" s="9"/>
     </row>
-    <row r="149" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="4:5">
       <c r="D149" s="8"/>
       <c r="E149" s="9"/>
     </row>
-    <row r="150" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="4:5">
       <c r="D150" s="8"/>
       <c r="E150" s="9"/>
     </row>
-    <row r="151" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="4:5">
       <c r="D151" s="8"/>
       <c r="E151" s="9"/>
     </row>
-    <row r="152" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="4:5">
       <c r="D152" s="8"/>
       <c r="E152" s="9"/>
     </row>
-    <row r="153" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="4:5">
       <c r="D153" s="8"/>
       <c r="E153" s="9"/>
     </row>
-    <row r="154" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="4:5">
       <c r="D154" s="8"/>
       <c r="E154" s="9"/>
     </row>
-    <row r="155" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="4:5">
       <c r="D155" s="8"/>
       <c r="E155" s="9"/>
     </row>
-    <row r="156" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="4:5">
       <c r="D156" s="8"/>
       <c r="E156" s="9"/>
     </row>
-    <row r="157" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="4:5">
       <c r="D157" s="8"/>
       <c r="E157" s="9"/>
     </row>
-    <row r="158" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="4:5">
       <c r="D158" s="8"/>
       <c r="E158" s="9"/>
     </row>
-    <row r="159" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="4:5">
       <c r="D159" s="8"/>
       <c r="E159" s="9"/>
     </row>
-    <row r="160" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="4:5">
       <c r="D160" s="8"/>
       <c r="E160" s="9"/>
     </row>
-    <row r="161" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="4:5">
       <c r="D161" s="8"/>
       <c r="E161" s="9"/>
     </row>
-    <row r="162" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="4:5">
       <c r="D162" s="8"/>
       <c r="E162" s="9"/>
     </row>
-    <row r="163" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="4:5">
       <c r="D163" s="8"/>
       <c r="E163" s="9"/>
     </row>
-    <row r="164" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="4:5">
       <c r="D164" s="8"/>
       <c r="E164" s="9"/>
     </row>
-    <row r="165" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="4:5">
       <c r="D165" s="8"/>
       <c r="E165" s="9"/>
     </row>
-    <row r="166" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="4:5">
       <c r="D166" s="8"/>
       <c r="E166" s="9"/>
     </row>
-    <row r="167" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="4:5">
       <c r="D167" s="8"/>
       <c r="E167" s="9"/>
     </row>
-    <row r="168" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="4:5">
       <c r="D168" s="8"/>
       <c r="E168" s="9"/>
     </row>
-    <row r="169" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="4:5">
       <c r="D169" s="8"/>
       <c r="E169" s="9"/>
     </row>
-    <row r="170" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="4:5">
       <c r="D170" s="8"/>
       <c r="E170" s="9"/>
     </row>
-    <row r="171" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="4:5">
       <c r="D171" s="8"/>
       <c r="E171" s="9"/>
     </row>
-    <row r="172" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="4:5">
       <c r="D172" s="8"/>
       <c r="E172" s="9"/>
     </row>
-    <row r="173" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="4:5">
       <c r="D173" s="8"/>
       <c r="E173" s="9"/>
     </row>
-    <row r="174" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="4:5">
       <c r="D174" s="8"/>
       <c r="E174" s="9"/>
     </row>
-    <row r="175" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="4:5">
       <c r="D175" s="8"/>
       <c r="E175" s="9"/>
     </row>
-    <row r="176" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="4:5">
       <c r="D176" s="8"/>
       <c r="E176" s="9"/>
     </row>
-    <row r="177" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="4:5">
       <c r="D177" s="8"/>
       <c r="E177" s="9"/>
     </row>
-    <row r="178" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="4:5">
       <c r="D178" s="8"/>
       <c r="E178" s="9"/>
     </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="4:5">
       <c r="D179" s="8"/>
       <c r="E179" s="9"/>
     </row>
-    <row r="180" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="4:5">
       <c r="D180" s="8"/>
       <c r="E180" s="9"/>
     </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="4:5">
       <c r="D181" s="8"/>
       <c r="E181" s="9"/>
     </row>
-    <row r="182" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="4:5">
       <c r="D182" s="8"/>
       <c r="E182" s="9"/>
     </row>
-    <row r="183" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="4:5">
       <c r="D183" s="8"/>
       <c r="E183" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K44"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="K55:L55 M53">
     <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="notEqual">
       <formula>0</formula>
@@ -3997,16 +3986,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" stopIfTrue="1" operator="containsText" text="fourth">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>NOT(ISERROR(SEARCH("fourth",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" stopIfTrue="1" operator="containsText" text="third">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>NOT(ISERROR(SEARCH("third",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" stopIfTrue="1" operator="containsText" text="second">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>NOT(ISERROR(SEARCH("second",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" stopIfTrue="1" operator="containsText" text="first">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>NOT(ISERROR(SEARCH("first",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4021,153 +4010,166 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <sheetData/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="24">
       <c r="A1" s="37" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="38">
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="38">
         <v>2</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="38">
         <v>3</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="38">
         <v>4</v>
       </c>
       <c r="B5" s="38"/>
       <c r="C5" s="38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="38">
         <v>5</v>
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="38">
         <v>6</v>
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="38">
         <v>7</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="38">
         <v>8</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="38">
         <v>9</v>
       </c>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="38">
         <v>10</v>
       </c>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="36" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>